<commit_message>
Commit on 28Dec with new changes
</commit_message>
<xml_diff>
--- a/data/Testdata.xlsx
+++ b/data/Testdata.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="169">
   <si>
     <t>Key</t>
   </si>
@@ -463,9 +463,6 @@
     <t>Junaid Tariq</t>
   </si>
   <si>
-    <t>3rd Lane William</t>
-  </si>
-  <si>
     <t>AdmType2</t>
   </si>
   <si>
@@ -497,6 +494,42 @@
   </si>
   <si>
     <t>firstNam</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>Mr</t>
+  </si>
+  <si>
+    <t>middleName</t>
+  </si>
+  <si>
+    <t>AutomationMiddleName</t>
+  </si>
+  <si>
+    <t>AddLine2</t>
+  </si>
+  <si>
+    <t>3rd Lane William Street</t>
+  </si>
+  <si>
+    <t>Brooklane</t>
+  </si>
+  <si>
+    <t>phone</t>
+  </si>
+  <si>
+    <t>mobile</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>jtariq@ucm.com.au</t>
+  </si>
+  <si>
+    <t>(08) 4356-7689</t>
   </si>
 </sst>
 </file>
@@ -556,7 +589,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -572,6 +605,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1901,10 +1935,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1915,7 +1949,7 @@
     <col min="4" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1923,132 +1957,183 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>157</v>
       </c>
       <c r="B2" s="6" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>156</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>128</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B6" s="6" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+      <c r="B17" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="B11" s="1" t="s">
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
+      <c r="B18" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B19" s="1" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="13" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B20" s="1" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="15" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="3"/>
-      <c r="B15" s="5"/>
-    </row>
-    <row r="16" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="3"/>
-      <c r="B16" s="4"/>
-    </row>
-    <row r="17" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="3"/>
-      <c r="B17" s="4"/>
-      <c r="D17" s="4"/>
-    </row>
-    <row r="18" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="3"/>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="3"/>
+      <c r="B21" s="5"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="3"/>
+      <c r="B22" s="4"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="3"/>
+      <c r="B23" s="4"/>
+      <c r="D23" s="4"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="3"/>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B17">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B23">
       <formula1>"','C:,'D:,'E:,'F:,"</formula1>
     </dataValidation>
   </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="B11" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2165,53 +2250,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_dlc_DocId xmlns="f7c95c21-70cf-4f55-a2aa-42a8ccf5f8e5">HRRKFX3D3EU6-345154152-145</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="f7c95c21-70cf-4f55-a2aa-42a8ccf5f8e5">
+      <Url>http://enterprisetfs.systemsltd.com/sites/SL-DBU/RUC/_layouts/15/DocIdRedir.aspx?ID=HRRKFX3D3EU6-345154152-145</Url>
+      <Description>HRRKFX3D3EU6-345154152-145</Description>
+    </_dlc_DocIdUrl>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2360,15 +2407,53 @@
 </file>
 
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_dlc_DocId xmlns="f7c95c21-70cf-4f55-a2aa-42a8ccf5f8e5">HRRKFX3D3EU6-345154152-145</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="f7c95c21-70cf-4f55-a2aa-42a8ccf5f8e5">
-      <Url>http://enterprisetfs.systemsltd.com/sites/SL-DBU/RUC/_layouts/15/DocIdRedir.aspx?ID=HRRKFX3D3EU6-345154152-145</Url>
-      <Description>HRRKFX3D3EU6-345154152-145</Description>
-    </_dlc_DocIdUrl>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2380,9 +2465,17 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{10B372F3-4FE9-46FF-BB1C-9BA2799EB127}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{162431BF-6DFE-4D42-A598-9B628181FC89}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="f7c95c21-70cf-4f55-a2aa-42a8ccf5f8e5"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2406,17 +2499,9 @@
 </file>
 
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{162431BF-6DFE-4D42-A598-9B628181FC89}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{10B372F3-4FE9-46FF-BB1C-9BA2799EB127}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="f7c95c21-70cf-4f55-a2aa-42a8ccf5f8e5"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Commit on 29Dec with new changes
</commit_message>
<xml_diff>
--- a/data/Testdata.xlsx
+++ b/data/Testdata.xlsx
@@ -12,17 +12,18 @@
     <sheet name="PermanentExtAgreement" sheetId="30" r:id="rId3"/>
     <sheet name="RespiteAgreement" sheetId="31" r:id="rId4"/>
     <sheet name="RespiteExtAgreement" sheetId="32" r:id="rId5"/>
-    <sheet name="UserCreation" sheetId="33" r:id="rId6"/>
-    <sheet name="MongoDetail" sheetId="27" r:id="rId7"/>
-    <sheet name="mail" sheetId="23" r:id="rId8"/>
+    <sheet name="UserCreation" sheetId="34" r:id="rId6"/>
+    <sheet name="UserCreation1" sheetId="33" r:id="rId7"/>
+    <sheet name="MongoDetail" sheetId="27" r:id="rId8"/>
+    <sheet name="mail" sheetId="23" r:id="rId9"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:D18"/>
+  <oleSize ref="A28:H49"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="212">
   <si>
     <t>Key</t>
   </si>
@@ -463,24 +464,6 @@
     <t>Junaid Tariq</t>
   </si>
   <si>
-    <t>AdmType2</t>
-  </si>
-  <si>
-    <t>Permanent / Extra Service</t>
-  </si>
-  <si>
-    <t>AdmType3</t>
-  </si>
-  <si>
-    <t>AdmType4</t>
-  </si>
-  <si>
-    <t>Respite</t>
-  </si>
-  <si>
-    <t>Respite / Extra Service</t>
-  </si>
-  <si>
     <t>setPropDischargeAdmDate</t>
   </si>
   <si>
@@ -530,6 +513,153 @@
   </si>
   <si>
     <t>(08) 4356-7689</t>
+  </si>
+  <si>
+    <t>residentId</t>
+  </si>
+  <si>
+    <t>999</t>
+  </si>
+  <si>
+    <t>gender</t>
+  </si>
+  <si>
+    <t>Not Stated</t>
+  </si>
+  <si>
+    <t>maritalStatus</t>
+  </si>
+  <si>
+    <t>Never Married</t>
+  </si>
+  <si>
+    <t>preferredLanguage</t>
+  </si>
+  <si>
+    <t>English</t>
+  </si>
+  <si>
+    <t>No Ethnicity</t>
+  </si>
+  <si>
+    <t>ethnicity</t>
+  </si>
+  <si>
+    <t>culturalIdentity</t>
+  </si>
+  <si>
+    <t>Australian Antarctic Territory</t>
+  </si>
+  <si>
+    <t>religion</t>
+  </si>
+  <si>
+    <t>Islam</t>
+  </si>
+  <si>
+    <t>enquirySource</t>
+  </si>
+  <si>
+    <t>Home</t>
+  </si>
+  <si>
+    <t>admissionTimeFrame</t>
+  </si>
+  <si>
+    <t>Completed Admission</t>
+  </si>
+  <si>
+    <t>pensionerNumber</t>
+  </si>
+  <si>
+    <t>1234567890</t>
+  </si>
+  <si>
+    <t>anACCClass</t>
+  </si>
+  <si>
+    <t>Class 6</t>
+  </si>
+  <si>
+    <t>residentCategory</t>
+  </si>
+  <si>
+    <t>Fully Supported</t>
+  </si>
+  <si>
+    <t>aCATStatus</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>aCATApprovalDate</t>
+  </si>
+  <si>
+    <t>16/12/2023</t>
+  </si>
+  <si>
+    <t>myAgedCareNumber</t>
+  </si>
+  <si>
+    <t>90909090</t>
+  </si>
+  <si>
+    <t>mediCareNumber</t>
+  </si>
+  <si>
+    <t>88888888888888</t>
+  </si>
+  <si>
+    <t>medicareCardExpiry</t>
+  </si>
+  <si>
+    <t>meansTestAssessment</t>
+  </si>
+  <si>
+    <t>Pending</t>
+  </si>
+  <si>
+    <t>mediCareNumber2</t>
+  </si>
+  <si>
+    <t>888</t>
+  </si>
+  <si>
+    <t>secondPreference</t>
+  </si>
+  <si>
+    <t>Barossa Hills Fleurieu</t>
+  </si>
+  <si>
+    <t>thirdPreference</t>
+  </si>
+  <si>
+    <t>Yorke &amp; North Central</t>
+  </si>
+  <si>
+    <t>extraServicePreference</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>catersToDementiaNeeds</t>
+  </si>
+  <si>
+    <t>roomPreference</t>
+  </si>
+  <si>
+    <t>Single</t>
+  </si>
+  <si>
+    <t>additionalServicePreference</t>
+  </si>
+  <si>
+    <t>88</t>
+  </si>
+  <si>
+    <t>8888888888</t>
   </si>
 </sst>
 </file>
@@ -589,7 +719,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -606,6 +736,10 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -890,7 +1024,7 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1935,10 +2069,371 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:C42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B43" sqref="B43"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="56.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="74.7109375" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="B35" s="8" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B11" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C44"/>
+  <sheetViews>
+    <sheetView topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1959,26 +2454,26 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1986,7 +2481,7 @@
         <v>128</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1994,15 +2489,15 @@
         <v>137</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -2015,130 +2510,292 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>131</v>
+        <v>163</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>136</v>
+        <v>165</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>153</v>
+        <v>167</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B22" s="1" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B25" s="1" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="B35" s="8" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B36" s="1" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="3"/>
-      <c r="B21" s="5"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="3"/>
-      <c r="B22" s="4"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="3"/>
-      <c r="B23" s="4"/>
-      <c r="D23" s="4"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="3"/>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="B38" s="6" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="B39" s="6" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="B40" s="6" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="B41" s="6" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="B42" s="6" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B43" s="11"/>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B44" s="11"/>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B23">
-      <formula1>"','C:,'D:,'E:,'F:,"</formula1>
-    </dataValidation>
-  </dataValidations>
   <hyperlinks>
     <hyperlink ref="B11" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -2188,7 +2845,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>

</xml_diff>

<commit_message>
Commit on 2nd Jan with new changes
</commit_message>
<xml_diff>
--- a/data/Testdata.xlsx
+++ b/data/Testdata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21510" windowHeight="7425" tabRatio="876" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21510" windowHeight="6420" tabRatio="876" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="20" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="232">
   <si>
     <t>Key</t>
   </si>
@@ -660,6 +660,66 @@
   </si>
   <si>
     <t>8888888888</t>
+  </si>
+  <si>
+    <t>representativeTitle</t>
+  </si>
+  <si>
+    <t>representativeFirstNam</t>
+  </si>
+  <si>
+    <t>representativeMiddleName</t>
+  </si>
+  <si>
+    <t>representativeLastName</t>
+  </si>
+  <si>
+    <t>representativeAddLine1</t>
+  </si>
+  <si>
+    <t>representativeAddLine2</t>
+  </si>
+  <si>
+    <t>representativeSetSuburb</t>
+  </si>
+  <si>
+    <t>representativePhone</t>
+  </si>
+  <si>
+    <t>representativeMobile</t>
+  </si>
+  <si>
+    <t>representativeEmail</t>
+  </si>
+  <si>
+    <t>representativeDrivingLicenseNo</t>
+  </si>
+  <si>
+    <t>repAutomationFirstName</t>
+  </si>
+  <si>
+    <t>repAutomationMiddleName</t>
+  </si>
+  <si>
+    <t>repAutomationLastName</t>
+  </si>
+  <si>
+    <t>Mrs Smith 98 Shirley Street</t>
+  </si>
+  <si>
+    <t>PIMPAMA QLD 4209</t>
+  </si>
+  <si>
+    <t>relationship</t>
+  </si>
+  <si>
+    <t>Cousin</t>
+  </si>
+  <si>
+    <t>Arrawarra Headland, New South Wales, 2456</t>
+  </si>
+  <si>
+    <t>Aarons Pass</t>
   </si>
 </sst>
 </file>
@@ -2069,15 +2129,15 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C42"/>
+  <dimension ref="A1:C54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B43" sqref="B43"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.42578125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="34" style="1" customWidth="1"/>
     <col min="2" max="2" width="56.42578125" style="1" customWidth="1"/>
     <col min="3" max="3" width="74.7109375" style="1" customWidth="1"/>
     <col min="4" max="16384" width="9.140625" style="1"/>
@@ -2419,12 +2479,112 @@
         <v>205</v>
       </c>
     </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="B43" s="6" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="B44" s="6" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="B45" s="6" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="B46" s="6" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="B47" s="6" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="B48" s="6" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="B49" s="6" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="B50" s="6" t="s">
+        <v>231</v>
+      </c>
+      <c r="C50" s="6" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="B51" s="6" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="B52" s="6" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="B53" s="9" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="B54" s="6" t="s">
+        <v>227</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B11" r:id="rId1"/>
+    <hyperlink ref="B53" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -2899,26 +3059,55 @@
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_dlc_DocId xmlns="f7c95c21-70cf-4f55-a2aa-42a8ccf5f8e5">HRRKFX3D3EU6-345154152-145</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="f7c95c21-70cf-4f55-a2aa-42a8ccf5f8e5">
-      <Url>http://enterprisetfs.systemsltd.com/sites/SL-DBU/RUC/_layouts/15/DocIdRedir.aspx?ID=HRRKFX3D3EU6-345154152-145</Url>
-      <Description>HRRKFX3D3EU6-345154152-145</Description>
-    </_dlc_DocIdUrl>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100209EC8D1B460E04EAE9C1B1C8AC8DB28" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b351c033c9c9815478ca7eb3b1834e90">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="f7c95c21-70cf-4f55-a2aa-42a8ccf5f8e5" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="cf3754e477bad867b7d6f1de6fcb6fff" ns2:_="">
     <xsd:import namespace="f7c95c21-70cf-4f55-a2aa-42a8ccf5f8e5"/>
@@ -3063,81 +3252,36 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_dlc_DocId xmlns="f7c95c21-70cf-4f55-a2aa-42a8ccf5f8e5">HRRKFX3D3EU6-345154152-145</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="f7c95c21-70cf-4f55-a2aa-42a8ccf5f8e5">
+      <Url>http://enterprisetfs.systemsltd.com/sites/SL-DBU/RUC/_layouts/15/DocIdRedir.aspx?ID=HRRKFX3D3EU6-345154152-145</Url>
+      <Description>HRRKFX3D3EU6-345154152-145</Description>
+    </_dlc_DocIdUrl>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1B3E90C9-3DD0-4640-A9E4-2EED702FC869}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{10B372F3-4FE9-46FF-BB1C-9BA2799EB127}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{162431BF-6DFE-4D42-A598-9B628181FC89}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="f7c95c21-70cf-4f55-a2aa-42a8ccf5f8e5"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A00C9E4A-1077-497A-BADB-01962963AFE9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3155,10 +3299,26 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{162431BF-6DFE-4D42-A598-9B628181FC89}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="f7c95c21-70cf-4f55-a2aa-42a8ccf5f8e5"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{10B372F3-4FE9-46FF-BB1C-9BA2799EB127}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1B3E90C9-3DD0-4640-A9E4-2EED702FC869}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Commit on 5th Jan with new changes
</commit_message>
<xml_diff>
--- a/data/Testdata.xlsx
+++ b/data/Testdata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21510" windowHeight="6420" tabRatio="876" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21510" windowHeight="7260" tabRatio="876" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="20" r:id="rId1"/>
@@ -2131,8 +2131,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="B50" sqref="B50"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3058,6 +3058,27 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_dlc_DocId xmlns="f7c95c21-70cf-4f55-a2aa-42a8ccf5f8e5">HRRKFX3D3EU6-345154152-145</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="f7c95c21-70cf-4f55-a2aa-42a8ccf5f8e5">
+      <Url>http://enterprisetfs.systemsltd.com/sites/SL-DBU/RUC/_layouts/15/DocIdRedir.aspx?ID=HRRKFX3D3EU6-345154152-145</Url>
+      <Description>HRRKFX3D3EU6-345154152-145</Description>
+    </_dlc_DocIdUrl>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
   <Receiver>
@@ -3107,7 +3128,7 @@
 </spe:Receivers>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100209EC8D1B460E04EAE9C1B1C8AC8DB28" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b351c033c9c9815478ca7eb3b1834e90">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="f7c95c21-70cf-4f55-a2aa-42a8ccf5f8e5" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="cf3754e477bad867b7d6f1de6fcb6fff" ns2:_="">
     <xsd:import namespace="f7c95c21-70cf-4f55-a2aa-42a8ccf5f8e5"/>
@@ -3252,28 +3273,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_dlc_DocId xmlns="f7c95c21-70cf-4f55-a2aa-42a8ccf5f8e5">HRRKFX3D3EU6-345154152-145</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="f7c95c21-70cf-4f55-a2aa-42a8ccf5f8e5">
-      <Url>http://enterprisetfs.systemsltd.com/sites/SL-DBU/RUC/_layouts/15/DocIdRedir.aspx?ID=HRRKFX3D3EU6-345154152-145</Url>
-      <Description>HRRKFX3D3EU6-345154152-145</Description>
-    </_dlc_DocIdUrl>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{162431BF-6DFE-4D42-A598-9B628181FC89}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="f7c95c21-70cf-4f55-a2aa-42a8ccf5f8e5"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1B3E90C9-3DD0-4640-A9E4-2EED702FC869}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{10B372F3-4FE9-46FF-BB1C-9BA2799EB127}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
@@ -3281,7 +3305,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A00C9E4A-1077-497A-BADB-01962963AFE9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3297,28 +3321,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{162431BF-6DFE-4D42-A598-9B628181FC89}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="f7c95c21-70cf-4f55-a2aa-42a8ccf5f8e5"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1B3E90C9-3DD0-4640-A9E4-2EED702FC869}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Commit on 6th Jan with new changes
</commit_message>
<xml_diff>
--- a/data/Testdata.xlsx
+++ b/data/Testdata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21510" windowHeight="7260" tabRatio="876" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21450" windowHeight="5130" tabRatio="876" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="20" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="mail" sheetId="23" r:id="rId9"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A28:H49"/>
+  <oleSize ref="A28:G42"/>
 </workbook>
 </file>
 
@@ -1084,7 +1084,7 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1243,8 +1243,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2131,8 +2131,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>